<commit_message>
search test cases added
</commit_message>
<xml_diff>
--- a/testData/OpenCartTestCases.xlsx
+++ b/testData/OpenCartTestCases.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abgoyal\Downloads\Open-Cart-App-Testing\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4347F3-049D-400E-B871-7306816CC8BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1C5D35-07B7-428F-8BB8-4E1B6A75C3DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Register" sheetId="2" r:id="rId2"/>
     <sheet name="Logout" sheetId="3" r:id="rId3"/>
+    <sheet name="Search" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Login!$A$1:$H$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Register!$A$1:$I$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Search!$A$1:$I$24</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="319">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -924,6 +926,354 @@
   </si>
   <si>
     <t>TC_LG_001</t>
+  </si>
+  <si>
+    <t>1. Search functionality should work correctly in all the supported environments</t>
+  </si>
+  <si>
+    <t>1. Enter any existing product name into the 'Search' text box field - &lt;Refer Test Data&gt;
+2. Click on the button having search icon (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. Open the Application URL in any supported browser</t>
+  </si>
+  <si>
+    <t>Validate the Search functionality in all the supported environments</t>
+  </si>
+  <si>
+    <t>(TS_005)
+Search Functionality</t>
+  </si>
+  <si>
+    <t>TC_SF_022</t>
+  </si>
+  <si>
+    <t>1. Proper UI adhering to the UI checklist should be displayed for the complete Search functionality</t>
+  </si>
+  <si>
+    <t>Validate the UI of Search functionality and Search page options</t>
+  </si>
+  <si>
+    <t>TC_SF_021</t>
+  </si>
+  <si>
+    <t>1. A proper Page Heading, Page URL and Page Title should be displayed for 'Search' page</t>
+  </si>
+  <si>
+    <t>1. Enter any existing product name into the 'Search' text box field - &lt;Refer Test Data&gt;
+2. Click on the button having search icon 
+3. Check the Page Heading, Page URL and Page Title of the 'Search' page</t>
+  </si>
+  <si>
+    <t>Validate Page Heading, Page URL and Page Title of the 'Search' page</t>
+  </si>
+  <si>
+    <t>TC_SF_020</t>
+  </si>
+  <si>
+    <t>1. User should be able to perform Search operation and select several options in the Search page using the Keyboard keys Tab and Enter</t>
+  </si>
+  <si>
+    <t>1. Press Tab and Enter keys to perform Search operation and select several options in the Search page (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>Validate we can use all the options of Search functionality using the Keybaord keys</t>
+  </si>
+  <si>
+    <t>TC_SF_019</t>
+  </si>
+  <si>
+    <t>1. Breakcrumb option should be working correctly</t>
+  </si>
+  <si>
+    <t>Product Name: iMac</t>
+  </si>
+  <si>
+    <t>1. Enter any existing product name into the 'Search' text box field - &lt;Refer Test Data&gt;
+2. Click on the button having search icon 
+3. Check whether the Breadcrumb option</t>
+  </si>
+  <si>
+    <t>Validate Breadcrumb of the 'Search' page</t>
+  </si>
+  <si>
+    <t>TC_SF_018</t>
+  </si>
+  <si>
+    <t>1. User should be navigated to 'Search' page</t>
+  </si>
+  <si>
+    <t>1. Click on 'Site Map' link in the footer options
+2. Click on the 'Search' link from the 'Site Map' page (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>Validate navigating to Search page from the Site Map page</t>
+  </si>
+  <si>
+    <t>TC_SF_017</t>
+  </si>
+  <si>
+    <t>1. Search box field and the button with 'Search' icon should be displayed on all the page of the Application</t>
+  </si>
+  <si>
+    <t>1. Navigate to all the pages of the Application (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>Validate 'Search' textbox field and the button having search icon are displayed on all the page of the Application</t>
+  </si>
+  <si>
+    <t>TC_SF_016</t>
+  </si>
+  <si>
+    <t>1. More than one product should be displayed in the search results page
+2. The selected number of products should be displayed in the current search page</t>
+  </si>
+  <si>
+    <t>Product Name: Mac</t>
+  </si>
+  <si>
+    <t>1. Enter the search criteria in the 'Search' text box field which can result in mutliple products - &lt;Refer Test Data&gt;
+2. Click on the button having search icon (Validate ER-1)
+3. Select the number of Products to be displayed from the 'Show' dropdown (Validate ER-2)</t>
+  </si>
+  <si>
+    <t>Validate the User can select how many produts can be displayed in the Search Results</t>
+  </si>
+  <si>
+    <t>TC_SF_015</t>
+  </si>
+  <si>
+    <t>1. More than one product should be displayed in the search results page
+2. Products are sorted according to the options selected in the 'Sort By' dropdown field</t>
+  </si>
+  <si>
+    <t>1. Enter the search criteria in the 'Search' text box field which can result in mutliple products - &lt;Refer Test Data&gt;
+2. Click on the button having search icon (Validate ER-1)
+3. Select serveral options from the 'Sort By' dropdown (Validate ER-2)</t>
+  </si>
+  <si>
+    <t>Validate User is able to sort the Products displayed in the Search Results</t>
+  </si>
+  <si>
+    <t>TC_SF_014</t>
+  </si>
+  <si>
+    <t>1. User should be navigated to the Product Compare Page</t>
+  </si>
+  <si>
+    <t>1. Enter any existing product name into the 'Search' text box field - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the 'Product Compare' link (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>Validate navigating to Product Compare Page from Search Results page</t>
+  </si>
+  <si>
+    <t>TC_SF_013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. More than one products should be displayed in the search results page
+2. Multiple product should be dislayed in the List view without any problems and all the options (Add to Cart, Wish List and Compare Product) are working. Also User should be able to navigate to Product Displaye Page of products by clicking on Images and Product Name. 
+3. Multiple product should be dislayed in the Grid view without any problems and all the options (Add to Cart, Wish List and Compare Product) are working. Also User should be able to navigate to Product Displaye Page of products by clicking on Images and Product Name. 
+</t>
+  </si>
+  <si>
+    <t>Search Criteria: Mac</t>
+  </si>
+  <si>
+    <t>1. Enter the search criteria in the 'Search' text box field which can result in mutliple products - &lt;Refer Test Data&gt;
+2. Click on the button having search icon (Validate ER-1)
+3. Select 'List' option  (Validate ER-2)
+4. Select 'Grid' option (Validate ER-3)</t>
+  </si>
+  <si>
+    <t>Validate List and Grid views when  multiple Products are displayed in the search results</t>
+  </si>
+  <si>
+    <t>TC_SF_012</t>
+  </si>
+  <si>
+    <t>1. Single product should be dislayed in the List view without any problems and all the options (Add to Cart, Wish List and Compare Product) are working 
+2. User should be navigated to the Product Display Page of the product
+3. Single product should be dislayed in the Grid view without any problems and all the options (Add to Cart, Wish List and Compare Product) are working 
+4. User should be navigated to the Product Display Page of the product</t>
+  </si>
+  <si>
+    <t>1. Enter any existing product name into the 'Search' text box field - &lt;Refer Test Data&gt;
+2. Click on the button having search icon 
+3. Select 'List' option  (Validate ER-1)
+4. Click on the Image of the Product and name of the product (Validate ER-2)
+5. Repeat Steps 1 to 2 and Select 'Grid' option (Validate ER-3)
+6. Click on the Image of the Product and name of the product (Validate ER-4)</t>
+  </si>
+  <si>
+    <t>Validate List and Grid views when only one Product is displayed in the search results</t>
+  </si>
+  <si>
+    <t>TC_SF_011</t>
+  </si>
+  <si>
+    <t>1. 'There is no product that matches the search criteria' should be displayed in the Search Results page
+2. Searched product should be displayed in the search results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Name: iMac
+Parent Category Name: Desktops
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Don't enter anything into the 'Search' text box field 
+2. Click on the button having search icon 
+3. Enter any Product Name into the 'Search Criteria' text box field - &lt;Refer Test Data&gt;
+4. Select the Parent category of the given Product Name into 'Category' dropdown field - &lt;Refer Test Data&gt;
+5. Click on 'Search' button (Validate ER-1)
+6. Select 'Search in subcategories' checkbox field
+7. Click on 'Search' button (Validate ER-2)
+</t>
+  </si>
+  <si>
+    <t>Validate Search by selecting  to search in subcategories</t>
+  </si>
+  <si>
+    <t>TC_SF_010</t>
+  </si>
+  <si>
+    <t>There is no product that matches the search criteria' should be displayed in the Search Results page</t>
+  </si>
+  <si>
+    <t>Product Name: iMac
+Wrong Category Name: PC</t>
+  </si>
+  <si>
+    <t>1. Don't enter anything into the 'Search' text box field 
+2. Click on the button having search icon 
+3. Enter any Product Name into the 'Search Criteria' text box field - &lt;Refer Test Data&gt;
+4. Select a wrong category in tthe 'Category' dropdown field - - &lt;Refer Test Data&gt;
+5. Click on 'Search' button (Validate ER-2)</t>
+  </si>
+  <si>
+    <t>Validate Search by selecting the category of product</t>
+  </si>
+  <si>
+    <t>TC_SF_009</t>
+  </si>
+  <si>
+    <t>Product should be successfully displayed in the search results.</t>
+  </si>
+  <si>
+    <t>Product Name: iMac
+Correct Category Name: Mac</t>
+  </si>
+  <si>
+    <t>1. Don't enter anything into the 'Search' text box field 
+2. Click on the button having search icon 
+3. Enter any Product Name into the 'Search Criteria' text box field - &lt;Refer Test Data&gt;
+4. Select the correct category of the given Product Name into 'Category' dropdown field - &lt;Refer Test Data&gt;
+5. Click on 'Search' button (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. Product having the given text in its description should be displayed in the search results</t>
+  </si>
+  <si>
+    <t>Text in Production description of iMac Product:  iLife</t>
+  </si>
+  <si>
+    <t>1. Don't enter anything into the 'Search' text box field 
+2. Click on the button having search icon 
+3. Enter any text from the Product Description into the 'Search Criteria' text box field - &lt;Refer Test Data&gt;
+4. Select 'Search in product descriptions' checkbox option
+5. Click on 'Search' button (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>Validate Search using the text from the product description</t>
+  </si>
+  <si>
+    <t>TC_SF_008</t>
+  </si>
+  <si>
+    <t>1. Searched product should be displayed in the search results</t>
+  </si>
+  <si>
+    <t>1. Don't enter anything into the 'Search' text box field 
+2. Click on the button having search icon 
+3. Enter any existing product name into the 'Search Criteria' text box field - &lt;Refer Test Data&gt;
+4. Click on 'Search' button (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>Validate searching using 'Search Criteria' field</t>
+  </si>
+  <si>
+    <t>TC_SF_007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Proper placeholder text is displayed in the below fields:
+- Search text box field
+- Search Criteria text box field
+</t>
+  </si>
+  <si>
+    <t>1. Don't enter anything into the 'Search' text box field 
+2. Click on the button having search icon (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>Validate all the fields in the Search functionality and Search page have placeholders</t>
+  </si>
+  <si>
+    <t>TC_SF_006</t>
+  </si>
+  <si>
+    <t>1. More than one products should be displayed in the search results page</t>
+  </si>
+  <si>
+    <t>1. Enter the search criteria in the 'Search' text box field which can result in mutliple products - &lt;Refer Test Data&gt;
+2. Click on the button having search icon (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>Validate searching by providing a search criteria which results in mulitple products</t>
+  </si>
+  <si>
+    <t>TC_SF_005</t>
+  </si>
+  <si>
+    <t>1. Open the Application URL in any supported browser
+2. Login to the Application</t>
+  </si>
+  <si>
+    <t>Validate searching for a product after login to the Application</t>
+  </si>
+  <si>
+    <t>TC_SF_004</t>
+  </si>
+  <si>
+    <t>1.'There is no product that matches the search criteria' should be displayed in the Search Results page</t>
+  </si>
+  <si>
+    <t>Validate searching without providing any Product Name</t>
+  </si>
+  <si>
+    <t>TC_SF_003</t>
+  </si>
+  <si>
+    <t>1. 'There is no product that matches the search criteria' should be displayed in the Search Results page</t>
+  </si>
+  <si>
+    <t>Product Name: Fitbit</t>
+  </si>
+  <si>
+    <t>1. Enter non existing product name into the 'Search' text box field - &lt;Refer Test Data&gt;
+2. Click on the button having search icon (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>Validate searching with a non existing Product Name</t>
+  </si>
+  <si>
+    <t>TC_SF_002</t>
+  </si>
+  <si>
+    <t>Validate searching with an existing Product Name</t>
+  </si>
+  <si>
+    <t>TC_SF_001</t>
   </si>
 </sst>
 </file>
@@ -1380,8 +1730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1960,8 +2310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE1D9543-8464-4E0F-BC28-34902DCECC11}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="E17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView topLeftCell="E14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -2552,8 +2902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39281F2E-46DF-4CF5-BA55-C9B1022784CD}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView topLeftCell="E5" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2871,4 +3221,680 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{950A7B87-2D5F-4CC5-B12F-3D902C025A90}">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E15" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17:H24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="28.88671875" customWidth="1"/>
+    <col min="4" max="4" width="33.44140625" customWidth="1"/>
+    <col min="5" max="5" width="56.33203125" customWidth="1"/>
+    <col min="6" max="6" width="31.6640625" customWidth="1"/>
+    <col min="7" max="7" width="45.6640625" customWidth="1"/>
+    <col min="8" max="8" width="29.44140625" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="50.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>318</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>317</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>294</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2" s="18"/>
+    </row>
+    <row r="3" spans="1:9" ht="50.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>316</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>315</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>314</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>313</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>312</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="I3" s="16"/>
+    </row>
+    <row r="4" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>310</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>299</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>309</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="I4" s="16"/>
+    </row>
+    <row r="5" spans="1:9" ht="50.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>308</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>307</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>306</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>294</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="I5" s="16"/>
+    </row>
+    <row r="6" spans="1:9" ht="63" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
+        <v>305</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>304</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>303</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="I6" s="16"/>
+    </row>
+    <row r="7" spans="1:9" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>301</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>300</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>299</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="I7" s="16"/>
+    </row>
+    <row r="8" spans="1:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>295</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>294</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="I8" s="16"/>
+    </row>
+    <row r="9" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>293</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>292</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>291</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="I9" s="16"/>
+    </row>
+    <row r="10" spans="1:9" ht="172.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>288</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>287</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="I10" s="16"/>
+    </row>
+    <row r="11" spans="1:9" ht="172.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="I11" s="16"/>
+    </row>
+    <row r="12" spans="1:9" ht="126" x14ac:dyDescent="0.3">
+      <c r="A12" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>276</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="I12" s="16"/>
+    </row>
+    <row r="13" spans="1:9" ht="151.19999999999999" x14ac:dyDescent="0.3">
+      <c r="A13" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>274</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="I13" s="16"/>
+    </row>
+    <row r="14" spans="1:9" ht="214.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>270</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>267</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="I14" s="16"/>
+    </row>
+    <row r="15" spans="1:9" ht="50.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="18" t="s">
+        <v>266</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>263</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="I15" s="16"/>
+    </row>
+    <row r="16" spans="1:9" ht="95.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="I16" s="16"/>
+    </row>
+    <row r="17" spans="1:9" ht="88.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="I17" s="16"/>
+    </row>
+    <row r="18" spans="1:9" ht="63" x14ac:dyDescent="0.3">
+      <c r="A18" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="I18" s="16"/>
+    </row>
+    <row r="19" spans="1:9" ht="37.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A19" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="I19" s="16"/>
+    </row>
+    <row r="20" spans="1:9" ht="50.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="I20" s="16"/>
+    </row>
+    <row r="21" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="I21" s="16"/>
+    </row>
+    <row r="22" spans="1:9" ht="63" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="I22" s="16"/>
+    </row>
+    <row r="23" spans="1:9" ht="50.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="18" t="s">
+        <v>232</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="I23" s="16"/>
+    </row>
+    <row r="24" spans="1:9" ht="50.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="I24" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>